<commit_message>
New requirements.txt and README.md
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45113.92894988995</v>
+        <v>45116.91341651211</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45113.92894989048</v>
+        <v>45116.91341651322</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -529,14 +529,14 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45113.92895041757</v>
+        <v>45116.91341999901</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45113.92895244476</v>
+        <v>45116.91342195809</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.175sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.169sec </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -567,14 +567,14 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45113.92895307147</v>
+        <v>45116.91342219352</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45113.92895446638</v>
+        <v>45116.91342400664</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.12sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.156sec </t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -603,14 +603,14 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45113.92895521122</v>
+        <v>45116.91342430653</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45113.92895726665</v>
+        <v>45116.91342512117</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.177sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.07sec </t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -641,14 +641,14 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45113.92895827443</v>
+        <v>45116.91342541348</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45113.92895869845</v>
+        <v>45116.91342563316</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.036sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.018sec </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -677,14 +677,14 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45113.92895905425</v>
+        <v>45116.91342593425</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45113.92896282946</v>
+        <v>45116.91342863093</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.326sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.232sec </t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -714,14 +714,14 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45113.92896342622</v>
+        <v>45116.91342901658</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45113.92896738547</v>
+        <v>45116.91343417042</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.342sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.445sec </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -751,14 +751,14 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45113.92896836705</v>
+        <v>45116.91343447495</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45113.92897580464</v>
+        <v>45116.9134392728</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.642sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.414sec </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -788,14 +788,14 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45113.92897625107</v>
+        <v>45116.91343968582</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45113.92898459172</v>
+        <v>45116.9134458843</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.72sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.535sec </t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>

<commit_message>
Separate utils from main package
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45116.91341651211</v>
+        <v>45130.66270084777</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45116.91341651322</v>
+        <v>45130.66270084898</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -529,14 +529,14 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45116.91341999901</v>
+        <v>45130.66270534682</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45116.91342195809</v>
+        <v>45130.66270877632</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.169sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.296sec </t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -567,14 +567,14 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45116.91342219352</v>
+        <v>45130.66270921857</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45116.91342400664</v>
+        <v>45130.66271368905</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.156sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.386sec </t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -603,14 +603,14 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45116.91342430653</v>
+        <v>45130.66271415927</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45116.91342512117</v>
+        <v>45130.66271602872</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.07sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.161sec </t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -641,14 +641,14 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45116.91342541348</v>
+        <v>45130.66271637068</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45116.91342563316</v>
+        <v>45130.66271653711</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.018sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.014sec </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -677,14 +677,14 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45116.91342593425</v>
+        <v>45130.66271706452</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45116.91342863093</v>
+        <v>45130.66272009206</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.232sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.261sec </t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -714,14 +714,14 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45116.91342901658</v>
+        <v>45130.66272048949</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45116.91343417042</v>
+        <v>45130.66272637997</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.445sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.508sec </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -751,14 +751,14 @@
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45116.91343447495</v>
+        <v>45130.66272676507</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45116.9134392728</v>
+        <v>45130.66273586931</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.414sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.786sec </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -788,14 +788,14 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45116.91343968582</v>
+        <v>45130.66273630778</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45116.9134458843</v>
+        <v>45130.66274638397</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">0d, 0hr, 0min, 0.535sec </t>
+          <t xml:space="preserve">0d, 0hr, 0min, 0.87sec </t>
         </is>
       </c>
       <c r="H10" t="inlineStr">

</xml_diff>